<commit_message>
update if tgl lahir
</commit_message>
<xml_diff>
--- a/public/excel/format_pbj/pbjelsyin1.xlsx
+++ b/public/excel/format_pbj/pbjelsyin1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\membership_laravel\public\excel\format_pbj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15804C3-9F97-4AC3-8A10-32B629DE4629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6E7D88-8C53-490B-919D-D2CB17C95AF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,7 +730,7 @@
     <t>Martapura, 17 Agustus 1985</t>
   </si>
   <si>
-    <t>Aek Nabara, Jakarta, 16 Desember 1985</t>
+    <t>Aek Nabara, 16 Desember 1985</t>
   </si>
 </sst>
 </file>
@@ -1215,9 +1215,9 @@
   </sheetPr>
   <dimension ref="A1:AG127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>